<commit_message>
update wat te doen
</commit_message>
<xml_diff>
--- a/overzicht met wat gedaan moet worden voor het verslag.xlsx
+++ b/overzicht met wat gedaan moet worden voor het verslag.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hendrik Jan\Documents\GitHub\EPO4B12\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -196,7 +191,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -254,7 +249,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -289,7 +284,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -466,7 +461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -477,15 +472,15 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -497,12 +492,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -510,7 +505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -518,12 +513,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
@@ -531,7 +526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -539,7 +534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -547,7 +542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
@@ -555,7 +550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
@@ -563,90 +558,90 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
+    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="3" t="s">
+    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>29</v>
       </c>

</xml_diff>